<commit_message>
first attempt completed for one cut
</commit_message>
<xml_diff>
--- a/simulated_data.xlsx
+++ b/simulated_data.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -376,7 +376,7 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>3605.475200000001</v>
+        <v>3667.430990000001</v>
       </c>
       <c r="B2">
         <v>1.402125977911055</v>
@@ -387,7 +387,7 @@
     </row>
     <row r="3">
       <c r="A3">
-        <v>2922.4127</v>
+        <v>2984.36849</v>
       </c>
       <c r="B3">
         <v>11.43002836359665</v>
@@ -398,7 +398,7 @@
     </row>
     <row r="4">
       <c r="A4">
-        <v>674.0998999999999</v>
+        <v>692.1148999999999</v>
       </c>
       <c r="B4">
         <v>10.80911589739844</v>
@@ -409,7 +409,7 @@
     </row>
     <row r="5">
       <c r="A5">
-        <v>5853.788</v>
+        <v>5871.803</v>
       </c>
       <c r="B5">
         <v>9.867354356683791</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="6">
       <c r="A6">
-        <v>1960.2504</v>
+        <v>2022.20619</v>
       </c>
       <c r="B6">
         <v>6.711032608058304</v>
@@ -431,7 +431,7 @@
     </row>
     <row r="7">
       <c r="A7">
-        <v>4567.6375</v>
+        <v>4629.59329</v>
       </c>
       <c r="B7">
         <v>7.751758998725563</v>
@@ -442,7 +442,7 @@
     </row>
     <row r="8">
       <c r="A8">
-        <v>329.0525</v>
+        <v>347.0675</v>
       </c>
       <c r="B8">
         <v>9.733060268685222</v>
@@ -453,7 +453,7 @@
     </row>
     <row r="9">
       <c r="A9">
-        <v>6198.8354</v>
+        <v>6216.8504</v>
       </c>
       <c r="B9">
         <v>10.07750778272748</v>
@@ -464,7 +464,7 @@
     </row>
     <row r="10">
       <c r="A10">
-        <v>5548.7467</v>
+        <v>5610.70249</v>
       </c>
       <c r="B10">
         <v>5.106852845288813</v>
@@ -475,7 +475,7 @@
     </row>
     <row r="11">
       <c r="A11">
-        <v>979.1411999999999</v>
+        <v>1041.09699</v>
       </c>
       <c r="B11">
         <v>9.308235140517354</v>
@@ -486,7 +486,7 @@
     </row>
     <row r="12">
       <c r="A12">
-        <v>5892.8101</v>
+        <v>5910.8251</v>
       </c>
       <c r="B12">
         <v>8.62972926069051</v>
@@ -497,7 +497,7 @@
     </row>
     <row r="13">
       <c r="A13">
-        <v>635.0778</v>
+        <v>653.0928</v>
       </c>
       <c r="B13">
         <v>7.873177503235638</v>
@@ -508,7 +508,7 @@
     </row>
     <row r="14">
       <c r="A14">
-        <v>5853.788</v>
+        <v>5915.74379</v>
       </c>
       <c r="B14">
         <v>2.5615228950046</v>
@@ -519,7 +519,7 @@
     </row>
     <row r="15">
       <c r="A15">
-        <v>674.0998999999999</v>
+        <v>736.0556899999999</v>
       </c>
       <c r="B15">
         <v>13.92321351682767</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="16">
       <c r="A16">
-        <v>4262.5962</v>
+        <v>4280.6112</v>
       </c>
       <c r="B16">
         <v>4.306655411608517</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="17">
       <c r="A17">
-        <v>2265.2917</v>
+        <v>2283.3067</v>
       </c>
       <c r="B17">
         <v>6.38427272439003</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="18">
       <c r="A18">
-        <v>4912.6849</v>
+        <v>4930.699900000001</v>
       </c>
       <c r="B18">
         <v>12.4599950904958</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="19">
       <c r="A19">
-        <v>1615.203</v>
+        <v>1633.218</v>
       </c>
       <c r="B19">
         <v>7.889897698536515</v>
@@ -574,7 +574,7 @@
     </row>
     <row r="20">
       <c r="A20">
-        <v>1286.1505</v>
+        <v>1348.10629</v>
       </c>
       <c r="B20">
         <v>6.673630793578923</v>
@@ -585,7 +585,7 @@
     </row>
     <row r="21">
       <c r="A21">
-        <v>5241.7374</v>
+        <v>5303.69319</v>
       </c>
       <c r="B21">
         <v>10.30259809689596</v>
@@ -596,7 +596,7 @@
     </row>
     <row r="22">
       <c r="A22">
-        <v>2617.3714</v>
+        <v>2635.3864</v>
       </c>
       <c r="B22">
         <v>6.800201285164803</v>
@@ -607,7 +607,7 @@
     </row>
     <row r="23">
       <c r="A23">
-        <v>3910.516499999999</v>
+        <v>3928.531499999999</v>
       </c>
       <c r="B23">
         <v>2.216097831260413</v>
@@ -618,7 +618,7 @@
     </row>
     <row r="24">
       <c r="A24">
-        <v>3910.516500000001</v>
+        <v>3972.472290000001</v>
       </c>
       <c r="B24">
         <v>11.12857661768794</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="25">
       <c r="A25">
-        <v>2617.3714</v>
+        <v>2679.32719</v>
       </c>
       <c r="B25">
         <v>2.381598450243473</v>
@@ -640,7 +640,7 @@
     </row>
     <row r="26">
       <c r="A26">
-        <v>1615.203</v>
+        <v>1677.15879</v>
       </c>
       <c r="B26">
         <v>2.060205020941794</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="27">
       <c r="A27">
-        <v>4912.6849</v>
+        <v>4974.64069</v>
       </c>
       <c r="B27">
         <v>4.577458583749831</v>
@@ -662,7 +662,7 @@
     </row>
     <row r="28">
       <c r="A28">
-        <v>979.1412</v>
+        <v>997.1562</v>
       </c>
       <c r="B28">
         <v>14.36199652310461</v>
@@ -673,7 +673,7 @@
     </row>
     <row r="29">
       <c r="A29">
-        <v>5548.7467</v>
+        <v>5566.7617</v>
       </c>
       <c r="B29">
         <v>12.81600432284176</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="30">
       <c r="A30">
-        <v>4239.569</v>
+        <v>4301.52479</v>
       </c>
       <c r="B30">
         <v>10.89899302227423</v>
@@ -695,7 +695,7 @@
     </row>
     <row r="31">
       <c r="A31">
-        <v>2288.3189</v>
+        <v>2350.27469</v>
       </c>
       <c r="B31">
         <v>4.260187649633735</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="32">
       <c r="A32">
-        <v>6198.835400000001</v>
+        <v>6260.791190000001</v>
       </c>
       <c r="B32">
         <v>7.993033485021442</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="33">
       <c r="A33">
-        <v>4567.6375</v>
+        <v>391.00829</v>
       </c>
       <c r="B33">
         <v>9.767404143698514</v>
@@ -728,7 +728,7 @@
     </row>
     <row r="34">
       <c r="A34">
-        <v>1960.2504</v>
+        <v>4585.6525</v>
       </c>
       <c r="B34">
         <v>8.263915817253292</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="35">
       <c r="A35">
-        <v>4545.594300000001</v>
+        <v>1978.2654</v>
       </c>
       <c r="B35">
         <v>5.289341134950519</v>
@@ -750,7 +750,7 @@
     </row>
     <row r="36">
       <c r="A36">
-        <v>1982.2936</v>
+        <v>4607.550090000001</v>
       </c>
       <c r="B36">
         <v>5.193924769293517</v>
@@ -761,7 +761,7 @@
     </row>
     <row r="37">
       <c r="A37">
-        <v>2265.2917</v>
+        <v>2044.24939</v>
       </c>
       <c r="B37">
         <v>3.518531526438892</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="38">
       <c r="A38">
-        <v>4262.5962</v>
+        <v>2327.24749</v>
       </c>
       <c r="B38">
         <v>12.54478178638965</v>
@@ -783,7 +783,7 @@
     </row>
     <row r="39">
       <c r="A39">
-        <v>1653.2411</v>
+        <v>4324.55199</v>
       </c>
       <c r="B39">
         <v>6.036846867762506</v>
@@ -794,7 +794,7 @@
     </row>
     <row r="40">
       <c r="A40">
-        <v>4874.6468</v>
+        <v>1671.2561</v>
       </c>
       <c r="B40">
         <v>3.91916290903464</v>
@@ -805,7 +805,7 @@
     </row>
     <row r="41">
       <c r="A41">
-        <v>306.0253</v>
+        <v>4892.6618</v>
       </c>
       <c r="B41">
         <v>1.865453130099922</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="42">
       <c r="A42">
-        <v>6221.8626</v>
+        <v>367.98109</v>
       </c>
       <c r="B42">
         <v>8.283902868162841</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="43">
       <c r="A43">
-        <v>635.0778</v>
+        <v>6283.81839</v>
       </c>
       <c r="B43">
         <v>5.686381690669805</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="44">
       <c r="A44">
-        <v>5892.810100000001</v>
+        <v>697.03359</v>
       </c>
       <c r="B44">
         <v>5.751517934724689</v>
@@ -849,7 +849,7 @@
     </row>
     <row r="45">
       <c r="A45">
-        <v>2288.3189</v>
+        <v>5954.765890000001</v>
       </c>
       <c r="B45">
         <v>5.667865811381489</v>
@@ -860,7 +860,7 @@
     </row>
     <row r="46">
       <c r="A46">
-        <v>4239.569</v>
+        <v>2306.3339</v>
       </c>
       <c r="B46">
         <v>14.70432431669906</v>
@@ -871,7 +871,7 @@
     </row>
     <row r="47">
       <c r="A47">
-        <v>2610.3391</v>
+        <v>4257.584</v>
       </c>
       <c r="B47">
         <v>6.674329224508256</v>
@@ -882,7 +882,7 @@
     </row>
     <row r="48">
       <c r="A48">
-        <v>3917.5488</v>
+        <v>2672.29489</v>
       </c>
       <c r="B48">
         <v>14.03565506171435</v>
@@ -893,7 +893,7 @@
     </row>
     <row r="49">
       <c r="A49">
-        <v>1982.2936</v>
+        <v>3979.50459</v>
       </c>
       <c r="B49">
         <v>12.50415098015219</v>
@@ -904,7 +904,7 @@
     </row>
     <row r="50">
       <c r="A50">
-        <v>4545.5943</v>
+        <v>2000.3086</v>
       </c>
       <c r="B50">
         <v>7.814556941390038</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="51">
       <c r="A51">
-        <v>3612.5075</v>
+        <v>4563.6093</v>
       </c>
       <c r="B51">
         <v>13.63885116158053</v>
@@ -926,7 +926,7 @@
     </row>
     <row r="52">
       <c r="A52">
-        <v>2915.3804</v>
+        <v>3630.5225</v>
       </c>
       <c r="B52">
         <v>10.70069581875578</v>
@@ -937,7 +937,7 @@
     </row>
     <row r="53">
       <c r="A53">
-        <v>1308.1937</v>
+        <v>2933.395399999999</v>
       </c>
       <c r="B53">
         <v>6.206627360079437</v>
@@ -948,7 +948,7 @@
     </row>
     <row r="54">
       <c r="A54">
-        <v>5219.6942</v>
+        <v>1326.2087</v>
       </c>
       <c r="B54">
         <v>3.22643582848832</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="55">
       <c r="A55">
-        <v>5241.7374</v>
+        <v>5237.7092</v>
       </c>
       <c r="B55">
         <v>14.4543857886456</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="56">
       <c r="A56">
-        <v>1286.1505</v>
+        <v>5259.7524</v>
       </c>
       <c r="B56">
         <v>12.51670508924872</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="57">
       <c r="A57">
-        <v>4874.6468</v>
+        <v>1304.1655</v>
       </c>
       <c r="B57">
         <v>2.896263035014272</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="58">
       <c r="A58">
-        <v>1653.2411</v>
+        <v>4936.60259</v>
       </c>
       <c r="B58">
         <v>14.76390654081479</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="59">
       <c r="A59">
-        <v>3260.4278</v>
+        <v>1715.19689</v>
       </c>
       <c r="B59">
         <v>13.83768974384293</v>
@@ -1014,7 +1014,7 @@
     </row>
     <row r="60">
       <c r="A60">
-        <v>3267.4601</v>
+        <v>3322.38359</v>
       </c>
       <c r="B60">
         <v>10.64085420966148</v>
@@ -1025,7 +1025,7 @@
     </row>
     <row r="61">
       <c r="A61">
-        <v>6527.8879</v>
+        <v>3329.41589</v>
       </c>
       <c r="B61">
         <v>2.630695700645447</v>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="62">
       <c r="A62">
-        <v>5547.762699999999</v>
+        <v>6545.9029</v>
       </c>
       <c r="B62">
         <v>9.514576449990273</v>
@@ -1047,7 +1047,7 @@
     </row>
     <row r="63">
       <c r="A63">
-        <v>980.1251999999999</v>
+        <v>5565.7777</v>
       </c>
       <c r="B63">
         <v>9.464815934654325</v>
@@ -1058,7 +1058,7 @@
     </row>
     <row r="64">
       <c r="A64">
-        <v>3917.5488</v>
+        <v>998.1401999999999</v>
       </c>
       <c r="B64">
         <v>3.792240146081895</v>
@@ -1069,7 +1069,7 @@
     </row>
     <row r="65">
       <c r="A65">
-        <v>2610.3391</v>
+        <v>3935.5638</v>
       </c>
       <c r="B65">
         <v>13.48286427510902</v>
@@ -1080,7 +1080,7 @@
     </row>
     <row r="66">
       <c r="A66">
-        <v>6527.887900000001</v>
+        <v>2628.3541</v>
       </c>
       <c r="B66">
         <v>9.718098845332861</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="67">
       <c r="A67">
-        <v>2915.3804</v>
+        <v>6589.843690000001</v>
       </c>
       <c r="B67">
         <v>5.352878645062447</v>
@@ -1102,7 +1102,7 @@
     </row>
     <row r="68">
       <c r="A68">
-        <v>3612.5075</v>
+        <v>2977.33619</v>
       </c>
       <c r="B68">
         <v>1.171910731587559</v>
@@ -1113,7 +1113,7 @@
     </row>
     <row r="69">
       <c r="A69">
-        <v>3267.4601</v>
+        <v>3674.46329</v>
       </c>
       <c r="B69">
         <v>1.612447910476476</v>
@@ -1124,7 +1124,7 @@
     </row>
     <row r="70">
       <c r="A70">
-        <v>3260.427799999999</v>
+        <v>3285.4751</v>
       </c>
       <c r="B70">
         <v>9.149751935619861</v>
@@ -1135,7 +1135,7 @@
     </row>
     <row r="71">
       <c r="A71">
-        <v>5219.6942</v>
+        <v>3278.442799999999</v>
       </c>
       <c r="B71">
         <v>14.99214413762093</v>
@@ -1146,7 +1146,7 @@
     </row>
     <row r="72">
       <c r="A72">
-        <v>1308.1937</v>
+        <v>5281.64999</v>
       </c>
       <c r="B72">
         <v>5.767604018095881</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="73">
       <c r="A73">
-        <v>980.1251999999999</v>
+        <v>1370.14949</v>
       </c>
       <c r="B73">
         <v>1.045445160940289</v>
@@ -1168,7 +1168,7 @@
     </row>
     <row r="74">
       <c r="A74">
-        <v>5547.7627</v>
+        <v>1042.08099</v>
       </c>
       <c r="B74">
         <v>11.3314286605455</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="75">
       <c r="A75">
-        <v>6221.862599999999</v>
+        <v>5609.71849</v>
       </c>
       <c r="B75">
         <v>4.739535705652088</v>
@@ -1190,7 +1190,7 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>2922.4127</v>
+        <v>6239.8776</v>
       </c>
       <c r="B76">
         <v>2.827977422159165</v>
@@ -1201,13 +1201,35 @@
     </row>
     <row r="77">
       <c r="A77">
-        <v>3605.475199999999</v>
+        <v>324.0403</v>
       </c>
       <c r="B77">
         <v>14.11988576920703</v>
       </c>
       <c r="C77">
         <v>37267547.98032111</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78">
+        <v>2940.4277</v>
+      </c>
+      <c r="B78">
+        <v>10.81613249657676</v>
+      </c>
+      <c r="C78">
+        <v>14411002.08812393</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79">
+        <v>3623.490199999999</v>
+      </c>
+      <c r="B79">
+        <v>2.481001087930053</v>
+      </c>
+      <c r="C79">
+        <v>44898948.86223367</v>
       </c>
     </row>
   </sheetData>

</xml_diff>